<commit_message>
update on 20210430 ch 8 en
</commit_message>
<xml_diff>
--- a/story/主线剧情/main/level_main_08-01_end.xlsx
+++ b/story/主线剧情/main/level_main_08-01_end.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
   <si>
     <t>zh_CN</t>
   </si>
@@ -22,6 +22,12 @@
     <t>ja_JP</t>
   </si>
   <si>
+    <t>en_US</t>
+  </si>
+  <si>
+    <t>ko_KR</t>
+  </si>
+  <si>
     <t xml:space="preserve">[name="感染者纠察队"] 呃......
 </t>
   </si>
@@ -231,6 +237,214 @@
   </si>
   <si>
     <t xml:space="preserve">[name="タルラ"] まったく、素晴らしい記憶力だことで。
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Infected Patrol Unit"] Ngh...
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] I didn’t cut off your hands! Pick yourself up!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Infected Patrol Unit"] ...Don’t you dare think this is over!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] I’ll cut out your tongue right here, then.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Infected Patrol Unit"] Eek! 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] ...Off he goes.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] Are you oka—
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] What have you done! Oh, God, Talulah... Look at what you’ve done! 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Talulah, we’ll have to transport the village in two days. Just look at what you’ve...! 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] You fought a patrolman! There’ll be hell to pay now! 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] Letting him beat you was even less of an idea. It’s getting late, and he’s on the run. If I kill him now, we’ll be long gone by the time the others find his remains.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] But that wouldn’t solve any of our problems. Once the patrol unit regroups, they’d still come looking for us. They might well be out to get revenge on us. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] And yet you did it! Now what do we do!? 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] Calm down. They’re looking for Infected. They still don’t know. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] ......
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Don’t know what?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] They don’t know what I’m about to do.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Hey... Talulah!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] It’s okay. Come on, I’ll walk you back. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] Your leg there... It will need special attention to heal.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Hah. So today’s the day you start helping me walk? Always thought I was still in good shape myself. Who’d’ve guessed I couldn’t outrun it?  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Talulah, there’s something I need to tell you.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] What is it?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Old Man"] Ah, good question. Heh, hahah, sorry, I don’t remember. Look at me now. Look at my memory...  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] ......
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="Talulah"] That’s some impressive forgetfulness, alright.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="감염자 감시팀"] 윽……
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 손목을 자르진 않았으니 어서 일어나!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="감염자 감시팀"] ……이대로 당할 줄 알고!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 흐응, 그 놈의 혀부터 잘라줘야 할 것 같네.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="감염자 감시팀"] 윽!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] ……도망쳤군.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 할아버지, 괜찮으세요?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 탈룰라, 대체 무슨 짓을 한 거냐! 네가 무슨 짓을 저질렀는지 알아!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 며칠 뒤면 다른 마을로 갈 수 있었는데 이런 짓을 저질렀으니……!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 놈들을 건드렸으니 큰 사달이 나고 말겠군!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 그렇다고 계속 이렇게 당할 수만은 없잖아요. 놈이 도망쳤으니 이미 늦었어요. 지금 가서 놈을 해치울게요, 다른 사람이 저자의 흔적을 발견했을 때 우린 이미 이곳에 없을 거예요.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 그렇다고 이렇게 도망치는 게 능사는 아니에요. 놈들이 일단 집결하면 우리를 찾아내는 건 물론, 복수하려 들지도 몰라요.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 그걸 알면서 그런 짓을 했으니…… 이제 어쩌면 좋단 말이냐!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 걱정하지 마세요. 저들이 찾는 건 감염자예요, 그리고 아직 저들이 모르는 게 있죠.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] ……
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 뭘 말이냐?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 이제부터 제가 뭘 할지를요.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 탈룰라……!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 괜찮을 거예요. 할아버지, 제가 모셔다 드릴게요.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 할아버지, 다리…… 아무래도 치료받으셔야 할 것 같아요.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 하아, 네게 부축받을 날이 올 줄이야. 평생 사지 멀쩡하게 살 줄 알았는데, 세월 앞에 장사 없구나.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 탈룰라, 네가 꼭 들어야 할 이야기가 있다.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 그게 뭔데요?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="할아버지"] 아, 그게 뭐였더라? 으음, 하하…… 미안하구나, 잊어버렸지 뭐냐. 나이를 먹으니 기억이 가물가물해서……
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] ……
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[name="탈룰라"] 아무래도 병원에 좀 가보셔야 할 것 같네요.
 </t>
   </si>
 </sst>
@@ -589,234 +803,402 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>